<commit_message>
Correction code SP (#28) f34ad5220e1dacba35eb369c2b98beaf6f7bfcb5
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-ror-location.xlsx
+++ b/ig/main/StructureDefinition-ror-location.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4674" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4673" uniqueCount="725">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-28T06:38:38+00:00</t>
+    <t>2023-05-10T10:36:42+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2065,9 +2065,6 @@
   </si>
   <si>
     <t>systemeGeodesique : Une identification du système de référence fixant les règles de mesure des positions géographiques (CoordonneeGeographique)</t>
-  </si>
-  <si>
-    <t>The extension can be further extended to include unique geolocation identifiers, confidence, altitude, etc.</t>
   </si>
   <si>
     <t>Location.position.modifierExtension</t>
@@ -15519,11 +15516,9 @@
         <v>662</v>
       </c>
       <c r="M120" t="s" s="2">
-        <v>654</v>
-      </c>
-      <c r="N120" t="s" s="2">
-        <v>663</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="N120" s="2"/>
       <c r="O120" s="2"/>
       <c r="P120" t="s" s="2">
         <v>72</v>
@@ -15587,7 +15582,7 @@
         <v>111</v>
       </c>
       <c r="AK120" t="s" s="2">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="AL120" t="s" s="2">
         <v>72</v>
@@ -15595,14 +15590,14 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="2">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121" t="s" s="2">
@@ -15624,10 +15619,10 @@
         <v>103</v>
       </c>
       <c r="L121" t="s" s="2">
+        <v>665</v>
+      </c>
+      <c r="M121" t="s" s="2">
         <v>666</v>
-      </c>
-      <c r="M121" t="s" s="2">
-        <v>667</v>
       </c>
       <c r="N121" t="s" s="2">
         <v>106</v>
@@ -15682,7 +15677,7 @@
         <v>72</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>73</v>
@@ -15705,10 +15700,10 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -15731,16 +15726,16 @@
         <v>72</v>
       </c>
       <c r="K122" t="s" s="2">
+        <v>669</v>
+      </c>
+      <c r="L122" t="s" s="2">
         <v>670</v>
       </c>
-      <c r="L122" t="s" s="2">
+      <c r="M122" t="s" s="2">
         <v>671</v>
       </c>
-      <c r="M122" t="s" s="2">
+      <c r="N122" t="s" s="2">
         <v>672</v>
-      </c>
-      <c r="N122" t="s" s="2">
-        <v>673</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" t="s" s="2">
@@ -15790,7 +15785,7 @@
         <v>72</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>80</v>
@@ -15805,7 +15800,7 @@
         <v>93</v>
       </c>
       <c r="AK122" t="s" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AL122" t="s" s="2">
         <v>72</v>
@@ -15813,10 +15808,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -15839,16 +15834,16 @@
         <v>72</v>
       </c>
       <c r="K123" t="s" s="2">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L123" t="s" s="2">
+        <v>675</v>
+      </c>
+      <c r="M123" t="s" s="2">
         <v>676</v>
       </c>
-      <c r="M123" t="s" s="2">
-        <v>677</v>
-      </c>
       <c r="N123" t="s" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O123" s="2"/>
       <c r="P123" t="s" s="2">
@@ -15898,7 +15893,7 @@
         <v>72</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>80</v>
@@ -15913,7 +15908,7 @@
         <v>93</v>
       </c>
       <c r="AK123" t="s" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AL123" t="s" s="2">
         <v>72</v>
@@ -15921,10 +15916,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
@@ -15947,16 +15942,16 @@
         <v>72</v>
       </c>
       <c r="K124" t="s" s="2">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L124" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="M124" t="s" s="2">
         <v>679</v>
       </c>
-      <c r="M124" t="s" s="2">
-        <v>680</v>
-      </c>
       <c r="N124" t="s" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="O124" s="2"/>
       <c r="P124" t="s" s="2">
@@ -16006,7 +16001,7 @@
         <v>72</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>73</v>
@@ -16021,7 +16016,7 @@
         <v>93</v>
       </c>
       <c r="AK124" t="s" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AL124" t="s" s="2">
         <v>72</v>
@@ -16029,10 +16024,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
@@ -16058,16 +16053,16 @@
         <v>359</v>
       </c>
       <c r="L125" t="s" s="2">
+        <v>681</v>
+      </c>
+      <c r="M125" t="s" s="2">
         <v>682</v>
       </c>
-      <c r="M125" t="s" s="2">
+      <c r="N125" t="s" s="2">
         <v>683</v>
       </c>
-      <c r="N125" t="s" s="2">
+      <c r="O125" t="s" s="2">
         <v>684</v>
-      </c>
-      <c r="O125" t="s" s="2">
-        <v>685</v>
       </c>
       <c r="P125" t="s" s="2">
         <v>72</v>
@@ -16116,7 +16111,7 @@
         <v>72</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>73</v>
@@ -16131,7 +16126,7 @@
         <v>364</v>
       </c>
       <c r="AK125" t="s" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AL125" t="s" s="2">
         <v>72</v>
@@ -16139,10 +16134,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -16165,19 +16160,19 @@
         <v>72</v>
       </c>
       <c r="K126" t="s" s="2">
+        <v>687</v>
+      </c>
+      <c r="L126" t="s" s="2">
         <v>688</v>
       </c>
-      <c r="L126" t="s" s="2">
+      <c r="M126" t="s" s="2">
         <v>689</v>
       </c>
-      <c r="M126" t="s" s="2">
+      <c r="N126" t="s" s="2">
         <v>690</v>
       </c>
-      <c r="N126" t="s" s="2">
+      <c r="O126" t="s" s="2">
         <v>691</v>
-      </c>
-      <c r="O126" t="s" s="2">
-        <v>692</v>
       </c>
       <c r="P126" t="s" s="2">
         <v>72</v>
@@ -16226,7 +16221,7 @@
         <v>72</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AG126" t="s" s="2">
         <v>73</v>
@@ -16241,7 +16236,7 @@
         <v>364</v>
       </c>
       <c r="AK126" t="s" s="2">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="AL126" t="s" s="2">
         <v>72</v>
@@ -16249,10 +16244,10 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -16278,13 +16273,13 @@
         <v>652</v>
       </c>
       <c r="L127" t="s" s="2">
+        <v>694</v>
+      </c>
+      <c r="M127" t="s" s="2">
         <v>695</v>
       </c>
-      <c r="M127" t="s" s="2">
+      <c r="N127" t="s" s="2">
         <v>696</v>
-      </c>
-      <c r="N127" t="s" s="2">
-        <v>697</v>
       </c>
       <c r="O127" s="2"/>
       <c r="P127" t="s" s="2">
@@ -16334,7 +16329,7 @@
         <v>72</v>
       </c>
       <c r="AF127" t="s" s="2">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="AG127" t="s" s="2">
         <v>73</v>
@@ -16349,7 +16344,7 @@
         <v>93</v>
       </c>
       <c r="AK127" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AL127" t="s" s="2">
         <v>72</v>
@@ -16357,10 +16352,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
@@ -16463,10 +16458,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
@@ -16571,14 +16566,14 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" t="s" s="2">
@@ -16600,10 +16595,10 @@
         <v>103</v>
       </c>
       <c r="L130" t="s" s="2">
+        <v>665</v>
+      </c>
+      <c r="M130" t="s" s="2">
         <v>666</v>
-      </c>
-      <c r="M130" t="s" s="2">
-        <v>667</v>
       </c>
       <c r="N130" t="s" s="2">
         <v>106</v>
@@ -16658,7 +16653,7 @@
         <v>72</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>73</v>
@@ -16681,10 +16676,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" t="s" s="2">
@@ -16710,10 +16705,10 @@
         <v>164</v>
       </c>
       <c r="L131" t="s" s="2">
+        <v>702</v>
+      </c>
+      <c r="M131" t="s" s="2">
         <v>703</v>
-      </c>
-      <c r="M131" t="s" s="2">
-        <v>704</v>
       </c>
       <c r="N131" t="s" s="2">
         <v>302</v>
@@ -16745,11 +16740,11 @@
         <v>156</v>
       </c>
       <c r="Y131" t="s" s="2">
+        <v>704</v>
+      </c>
+      <c r="Z131" t="s" s="2">
         <v>705</v>
       </c>
-      <c r="Z131" t="s" s="2">
-        <v>706</v>
-      </c>
       <c r="AA131" t="s" s="2">
         <v>72</v>
       </c>
@@ -16766,7 +16761,7 @@
         <v>72</v>
       </c>
       <c r="AF131" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AG131" t="s" s="2">
         <v>73</v>
@@ -16781,7 +16776,7 @@
         <v>93</v>
       </c>
       <c r="AK131" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AL131" t="s" s="2">
         <v>72</v>
@@ -16789,10 +16784,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -16818,10 +16813,10 @@
         <v>316</v>
       </c>
       <c r="L132" t="s" s="2">
+        <v>707</v>
+      </c>
+      <c r="M132" t="s" s="2">
         <v>708</v>
-      </c>
-      <c r="M132" t="s" s="2">
-        <v>709</v>
       </c>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -16872,7 +16867,7 @@
         <v>72</v>
       </c>
       <c r="AF132" t="s" s="2">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AG132" t="s" s="2">
         <v>73</v>
@@ -16887,7 +16882,7 @@
         <v>93</v>
       </c>
       <c r="AK132" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AL132" t="s" s="2">
         <v>72</v>
@@ -16895,10 +16890,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -16921,13 +16916,13 @@
         <v>72</v>
       </c>
       <c r="K133" t="s" s="2">
+        <v>710</v>
+      </c>
+      <c r="L133" t="s" s="2">
         <v>711</v>
       </c>
-      <c r="L133" t="s" s="2">
+      <c r="M133" t="s" s="2">
         <v>712</v>
-      </c>
-      <c r="M133" t="s" s="2">
-        <v>713</v>
       </c>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -16978,7 +16973,7 @@
         <v>72</v>
       </c>
       <c r="AF133" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="AG133" t="s" s="2">
         <v>73</v>
@@ -16993,7 +16988,7 @@
         <v>93</v>
       </c>
       <c r="AK133" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AL133" t="s" s="2">
         <v>72</v>
@@ -17001,10 +16996,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -17027,13 +17022,13 @@
         <v>72</v>
       </c>
       <c r="K134" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="L134" t="s" s="2">
+        <v>714</v>
+      </c>
+      <c r="M134" t="s" s="2">
         <v>715</v>
-      </c>
-      <c r="M134" t="s" s="2">
-        <v>716</v>
       </c>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
@@ -17084,7 +17079,7 @@
         <v>72</v>
       </c>
       <c r="AF134" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="AG134" t="s" s="2">
         <v>73</v>
@@ -17099,7 +17094,7 @@
         <v>93</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AL134" t="s" s="2">
         <v>72</v>
@@ -17107,10 +17102,10 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B135" t="s" s="2">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" t="s" s="2">
@@ -17136,10 +17131,10 @@
         <v>96</v>
       </c>
       <c r="L135" t="s" s="2">
+        <v>717</v>
+      </c>
+      <c r="M135" t="s" s="2">
         <v>718</v>
-      </c>
-      <c r="M135" t="s" s="2">
-        <v>719</v>
       </c>
       <c r="N135" t="s" s="2">
         <v>302</v>
@@ -17192,7 +17187,7 @@
         <v>72</v>
       </c>
       <c r="AF135" t="s" s="2">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="AG135" t="s" s="2">
         <v>73</v>
@@ -17215,10 +17210,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B136" t="s" s="2">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" t="s" s="2">
@@ -17241,19 +17236,19 @@
         <v>72</v>
       </c>
       <c r="K136" t="s" s="2">
+        <v>720</v>
+      </c>
+      <c r="L136" t="s" s="2">
         <v>721</v>
       </c>
-      <c r="L136" t="s" s="2">
+      <c r="M136" t="s" s="2">
         <v>722</v>
       </c>
-      <c r="M136" t="s" s="2">
+      <c r="N136" t="s" s="2">
+        <v>690</v>
+      </c>
+      <c r="O136" t="s" s="2">
         <v>723</v>
-      </c>
-      <c r="N136" t="s" s="2">
-        <v>691</v>
-      </c>
-      <c r="O136" t="s" s="2">
-        <v>724</v>
       </c>
       <c r="P136" t="s" s="2">
         <v>72</v>
@@ -17302,7 +17297,7 @@
         <v>72</v>
       </c>
       <c r="AF136" t="s" s="2">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="AG136" t="s" s="2">
         <v>73</v>
@@ -17317,7 +17312,7 @@
         <v>364</v>
       </c>
       <c r="AK136" t="s" s="2">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="AL136" t="s" s="2">
         <v>72</v>

</xml_diff>